<commit_message>
gdesc done (95%) READ DESCRIPTION
rooms now have descriptions, and they are loaded (Use #define DEBUG in game_reader.c to see it).
</commit_message>
<xml_diff>
--- a/I2_Gant_Saul_Lopez_Fernando_Mijangos.xlsx
+++ b/I2_Gant_Saul_Lopez_Fernando_Mijangos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\saul\Pprog_conversation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8061590-5D5B-47B9-948E-84019AA123F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FE9906-8149-4ED3-85D4-D71194CFD5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{05C49126-5558-4AD1-950B-328547F3A5DA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="92">
   <si>
     <t>CRONOGRAMA I2</t>
   </si>
@@ -290,13 +290,25 @@
   </si>
   <si>
     <t>DESGLOSE</t>
+  </si>
+  <si>
+    <t>Leyenda</t>
+  </si>
+  <si>
+    <t>Objetivo a medias</t>
+  </si>
+  <si>
+    <t>Objetivo completo</t>
+  </si>
+  <si>
+    <t>Objetivo no empezado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,8 +316,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -414,8 +433,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -714,11 +739,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -905,6 +943,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1231,10 +1287,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:Y56"/>
+  <dimension ref="A1:AB56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="73" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="73" workbookViewId="0">
+      <selection activeCell="AB35" sqref="AB35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1244,10 +1300,12 @@
     <col min="3" max="3" width="37.6328125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="5" style="3" customWidth="1"/>
     <col min="6" max="25" width="2.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="10.90625" style="3"/>
+    <col min="26" max="27" width="10.90625" style="3"/>
+    <col min="28" max="28" width="19.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
@@ -1276,7 +1334,7 @@
       <c r="X1" s="50"/>
       <c r="Y1" s="51"/>
     </row>
-    <row r="2" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="52" t="s">
         <v>87</v>
       </c>
@@ -1311,7 +1369,7 @@
       <c r="X2" s="65"/>
       <c r="Y2" s="66"/>
     </row>
-    <row r="3" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A3" s="54"/>
       <c r="B3" s="55"/>
       <c r="C3" s="59"/>
@@ -1345,8 +1403,12 @@
       <c r="W3" s="65"/>
       <c r="X3" s="65"/>
       <c r="Y3" s="66"/>
-    </row>
-    <row r="4" spans="1:25" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AA3" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB3" s="68"/>
+    </row>
+    <row r="4" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="56"/>
       <c r="B4" s="57"/>
       <c r="C4" s="60"/>
@@ -1416,8 +1478,14 @@
       <c r="Y4" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA4" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1453,8 +1521,14 @@
       <c r="W5" s="8"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="2"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA5" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
@@ -1492,8 +1566,14 @@
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="2"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AA6" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB6" s="71" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
@@ -1503,7 +1583,7 @@
       <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="70" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="1"/>
@@ -1530,7 +1610,7 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="2"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1540,7 +1620,7 @@
       <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="70" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="1"/>
@@ -1567,7 +1647,7 @@
       <c r="X8" s="1"/>
       <c r="Y8" s="2"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
@@ -1577,7 +1657,7 @@
       <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="70" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="1"/>
@@ -1604,7 +1684,7 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="2"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
@@ -1614,7 +1694,7 @@
       <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="70" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="1"/>
@@ -1643,7 +1723,7 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="11" t="s">
         <v>15</v>
       </c>
@@ -1653,7 +1733,7 @@
       <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="70" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="1"/>
@@ -1682,7 +1762,7 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="2"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
@@ -1692,7 +1772,7 @@
       <c r="C12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="70" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="1"/>
@@ -1723,7 +1803,7 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
@@ -1733,7 +1813,7 @@
       <c r="C13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="70" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="1"/>
@@ -1766,7 +1846,7 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="2"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>23</v>
       </c>
@@ -1803,7 +1883,7 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -1842,7 +1922,7 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="2"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
@@ -2211,7 +2291,7 @@
       <c r="X24" s="1"/>
       <c r="Y24" s="2"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="15" t="s">
         <v>36</v>
       </c>
@@ -2221,7 +2301,7 @@
       <c r="C25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="70" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="1"/>
@@ -2248,7 +2328,7 @@
       <c r="X25" s="1"/>
       <c r="Y25" s="2"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="17" t="s">
         <v>38</v>
       </c>
@@ -2258,7 +2338,7 @@
       <c r="C26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="70" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="1"/>
@@ -2285,7 +2365,7 @@
       <c r="X26" s="1"/>
       <c r="Y26" s="2"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
         <v>38</v>
       </c>
@@ -2370,18 +2450,22 @@
       <c r="B29" s="18">
         <v>4</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="1"/>
+      <c r="D29" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="36" t="s">
+        <v>12</v>
+      </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
+      <c r="J29" s="18" t="s">
+        <v>9</v>
+      </c>
       <c r="K29" s="18" t="s">
         <v>8</v>
       </c>
@@ -2402,7 +2486,7 @@
       <c r="X29" s="1"/>
       <c r="Y29" s="2"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="19" t="s">
         <v>43</v>
       </c>
@@ -2412,7 +2496,7 @@
       <c r="C30" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="70" t="s">
         <v>12</v>
       </c>
       <c r="E30" s="1"/>
@@ -2439,7 +2523,7 @@
       <c r="X30" s="1"/>
       <c r="Y30" s="2"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="21" t="s">
         <v>45</v>
       </c>
@@ -2449,7 +2533,7 @@
       <c r="C31" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="70" t="s">
         <v>12</v>
       </c>
       <c r="E31" s="1"/>
@@ -2476,7 +2560,7 @@
       <c r="X31" s="1"/>
       <c r="Y31" s="2"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A32" s="23" t="s">
         <v>47</v>
       </c>
@@ -2661,7 +2745,7 @@
       <c r="X36" s="1"/>
       <c r="Y36" s="2"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="29" t="s">
         <v>56</v>
       </c>
@@ -2671,7 +2755,7 @@
       <c r="C37" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="70" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="1"/>
@@ -2679,14 +2763,14 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
+      <c r="J37" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
-      <c r="O37" s="30" t="s">
-        <v>8</v>
-      </c>
+      <c r="O37" s="1"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
@@ -2698,7 +2782,7 @@
       <c r="X37" s="1"/>
       <c r="Y37" s="2"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="29" t="s">
         <v>56</v>
       </c>
@@ -2708,7 +2792,7 @@
       <c r="C38" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="70" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="1"/>
@@ -2716,17 +2800,15 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
+      <c r="J38" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
-      <c r="O38" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="P38" s="30" t="s">
-        <v>8</v>
-      </c>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
@@ -2737,7 +2819,7 @@
       <c r="X38" s="1"/>
       <c r="Y38" s="2"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="29" t="s">
         <v>56</v>
       </c>
@@ -2747,7 +2829,7 @@
       <c r="C39" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="70" t="s">
         <v>12</v>
       </c>
       <c r="E39" s="1"/>
@@ -2755,15 +2837,15 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
+      <c r="J39" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
-      <c r="P39" s="30" t="s">
-        <v>8</v>
-      </c>
+      <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
@@ -2774,7 +2856,7 @@
       <c r="X39" s="1"/>
       <c r="Y39" s="2"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A40" s="29" t="s">
         <v>56</v>
       </c>
@@ -2823,7 +2905,7 @@
       <c r="C41" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="36" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="1"/>
@@ -2831,7 +2913,9 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
+      <c r="J41" s="32" t="s">
+        <v>8</v>
+      </c>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -2839,9 +2923,7 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
-      <c r="R41" s="32" t="s">
-        <v>8</v>
-      </c>
+      <c r="R41" s="1"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
@@ -2850,7 +2932,7 @@
       <c r="X41" s="1"/>
       <c r="Y41" s="2"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="31" t="s">
         <v>61</v>
       </c>
@@ -2860,7 +2942,7 @@
       <c r="C42" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="70" t="s">
         <v>12</v>
       </c>
       <c r="E42" s="1"/>
@@ -2868,7 +2950,9 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
+      <c r="J42" s="32" t="s">
+        <v>8</v>
+      </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -2876,12 +2960,8 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
-      <c r="R42" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="S42" s="32" t="s">
-        <v>8</v>
-      </c>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
@@ -2889,7 +2969,7 @@
       <c r="X42" s="1"/>
       <c r="Y42" s="2"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A43" s="33" t="s">
         <v>64</v>
       </c>
@@ -2965,7 +3045,7 @@
       <c r="X44" s="1"/>
       <c r="Y44" s="2"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="33" t="s">
         <v>64</v>
       </c>
@@ -2975,23 +3055,25 @@
       <c r="C45" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="1"/>
+      <c r="D45" s="70" t="s">
+        <v>12</v>
+      </c>
       <c r="E45" s="1" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
+      <c r="J45" s="34" t="s">
+        <v>8</v>
+      </c>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
-      <c r="P45" s="34" t="s">
-        <v>9</v>
-      </c>
+      <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
@@ -3002,7 +3084,7 @@
       <c r="X45" s="1"/>
       <c r="Y45" s="2"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A46" s="33" t="s">
         <v>64</v>
       </c>
@@ -3378,7 +3460,8 @@
     </row>
     <row r="56" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="A1:Y1"/>
     <mergeCell ref="A2:B4"/>
     <mergeCell ref="C2:C4"/>

</xml_diff>

<commit_message>
Space_tester done + Started to use ID_ERROR
NO VUEVLVO A HACER UN TESTER DE MAS DE 20 FUNCIONES
</commit_message>
<xml_diff>
--- a/I2_Gant_Saul_Lopez_Fernando_Mijangos.xlsx
+++ b/I2_Gant_Saul_Lopez_Fernando_Mijangos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\saul\Pprog_conversation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fernandpo\cosa_uni\proyecto_program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B2371A-6F73-40F1-B04F-659F961FDBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177BF8FB-25FA-42D8-A833-F9016525845C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" xr2:uid="{05C49126-5558-4AD1-950B-328547F3A5DA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{05C49126-5558-4AD1-950B-328547F3A5DA}"/>
   </bookViews>
   <sheets>
     <sheet name="DIAGRAMA DE GANTT" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="92">
   <si>
     <t>CRONOGRAMA I2</t>
   </si>
@@ -988,9 +988,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1028,7 +1028,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1134,7 +1134,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1276,7 +1276,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1289,23 +1289,23 @@
   </sheetPr>
   <dimension ref="A1:AB56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="73" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="73" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="1.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="5" style="3" customWidth="1"/>
-    <col min="6" max="25" width="2.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="10.90625" style="3"/>
-    <col min="28" max="28" width="19.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.90625" style="3"/>
+    <col min="6" max="25" width="2.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="10.88671875" style="3"/>
+    <col min="28" max="28" width="19.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="25.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -1334,7 +1334,7 @@
       <c r="X1" s="56"/>
       <c r="Y1" s="57"/>
     </row>
-    <row r="2" spans="1:28" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:28" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="58" t="s">
         <v>87</v>
       </c>
@@ -1369,7 +1369,7 @@
       <c r="X2" s="71"/>
       <c r="Y2" s="72"/>
     </row>
-    <row r="3" spans="1:28" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="60"/>
       <c r="B3" s="61"/>
       <c r="C3" s="65"/>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="AB3" s="54"/>
     </row>
-    <row r="4" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="62"/>
       <c r="B4" s="63"/>
       <c r="C4" s="66"/>
@@ -1485,7 +1485,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
@@ -1610,7 +1610,7 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="2"/>
     </row>
-    <row r="8" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1647,7 +1647,7 @@
       <c r="X8" s="1"/>
       <c r="Y8" s="2"/>
     </row>
-    <row r="9" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
@@ -1684,7 +1684,7 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="2"/>
     </row>
-    <row r="10" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
@@ -1723,7 +1723,7 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>15</v>
       </c>
@@ -1762,7 +1762,7 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="2"/>
     </row>
-    <row r="12" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
@@ -1803,7 +1803,7 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
@@ -1846,7 +1846,7 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="2"/>
     </row>
-    <row r="14" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>23</v>
       </c>
@@ -1885,7 +1885,7 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -1924,7 +1924,7 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="2"/>
     </row>
-    <row r="16" spans="1:28" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
@@ -1963,7 +1963,7 @@
       <c r="X16" s="1"/>
       <c r="Y16" s="2"/>
     </row>
-    <row r="17" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
         <v>23</v>
       </c>
@@ -2000,7 +2000,7 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>23</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
@@ -2078,7 +2078,7 @@
       <c r="X19" s="1"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>29</v>
       </c>
@@ -2139,7 +2139,7 @@
       </c>
       <c r="Y20" s="2"/>
     </row>
-    <row r="21" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>29</v>
       </c>
@@ -2176,7 +2176,7 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="2"/>
     </row>
-    <row r="22" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>29</v>
       </c>
@@ -2213,7 +2213,7 @@
       <c r="X22" s="1"/>
       <c r="Y22" s="2"/>
     </row>
-    <row r="23" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>29</v>
       </c>
@@ -2250,7 +2250,7 @@
       <c r="X23" s="1"/>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>29</v>
       </c>
@@ -2287,7 +2287,7 @@
       <c r="X24" s="1"/>
       <c r="Y24" s="2"/>
     </row>
-    <row r="25" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>36</v>
       </c>
@@ -2324,7 +2324,7 @@
       <c r="X25" s="1"/>
       <c r="Y25" s="2"/>
     </row>
-    <row r="26" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
         <v>38</v>
       </c>
@@ -2361,7 +2361,7 @@
       <c r="X26" s="1"/>
       <c r="Y26" s="2"/>
     </row>
-    <row r="27" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
         <v>38</v>
       </c>
@@ -2400,7 +2400,7 @@
       <c r="X27" s="1"/>
       <c r="Y27" s="2"/>
     </row>
-    <row r="28" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="17" t="s">
         <v>38</v>
       </c>
@@ -2439,7 +2439,7 @@
       <c r="X28" s="1"/>
       <c r="Y28" s="2"/>
     </row>
-    <row r="29" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
         <v>38</v>
       </c>
@@ -2482,7 +2482,7 @@
       <c r="X29" s="1"/>
       <c r="Y29" s="2"/>
     </row>
-    <row r="30" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="19" t="s">
         <v>43</v>
       </c>
@@ -2519,7 +2519,7 @@
       <c r="X30" s="1"/>
       <c r="Y30" s="2"/>
     </row>
-    <row r="31" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="21" t="s">
         <v>45</v>
       </c>
@@ -2556,7 +2556,7 @@
       <c r="X31" s="1"/>
       <c r="Y31" s="2"/>
     </row>
-    <row r="32" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A32" s="23" t="s">
         <v>47</v>
       </c>
@@ -2593,7 +2593,7 @@
       <c r="X32" s="1"/>
       <c r="Y32" s="2"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="23" t="s">
         <v>47</v>
       </c>
@@ -2630,7 +2630,7 @@
       <c r="X33" s="1"/>
       <c r="Y33" s="2"/>
     </row>
-    <row r="34" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
         <v>50</v>
       </c>
@@ -2667,7 +2667,7 @@
       <c r="X34" s="1"/>
       <c r="Y34" s="2"/>
     </row>
-    <row r="35" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>52</v>
       </c>
@@ -2704,7 +2704,7 @@
       <c r="X35" s="1"/>
       <c r="Y35" s="2"/>
     </row>
-    <row r="36" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="27" t="s">
         <v>54</v>
       </c>
@@ -2741,7 +2741,7 @@
       <c r="X36" s="1"/>
       <c r="Y36" s="2"/>
     </row>
-    <row r="37" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="29" t="s">
         <v>56</v>
       </c>
@@ -2778,7 +2778,7 @@
       <c r="X37" s="1"/>
       <c r="Y37" s="2"/>
     </row>
-    <row r="38" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="29" t="s">
         <v>56</v>
       </c>
@@ -2815,7 +2815,7 @@
       <c r="X38" s="1"/>
       <c r="Y38" s="2"/>
     </row>
-    <row r="39" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="29" t="s">
         <v>56</v>
       </c>
@@ -2852,7 +2852,7 @@
       <c r="X39" s="1"/>
       <c r="Y39" s="2"/>
     </row>
-    <row r="40" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="29" t="s">
         <v>56</v>
       </c>
@@ -2862,10 +2862,12 @@
       <c r="C40" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="1"/>
+      <c r="D40" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="50" t="s">
+        <v>12</v>
+      </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -2876,12 +2878,8 @@
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
-      <c r="P40" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q40" s="30" t="s">
-        <v>8</v>
-      </c>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
@@ -2891,7 +2889,7 @@
       <c r="X40" s="1"/>
       <c r="Y40" s="2"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A41" s="31" t="s">
         <v>61</v>
       </c>
@@ -2928,7 +2926,7 @@
       <c r="X41" s="1"/>
       <c r="Y41" s="2"/>
     </row>
-    <row r="42" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="31" t="s">
         <v>61</v>
       </c>
@@ -2965,7 +2963,7 @@
       <c r="X42" s="1"/>
       <c r="Y42" s="2"/>
     </row>
-    <row r="43" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A43" s="33" t="s">
         <v>64</v>
       </c>
@@ -3004,7 +3002,7 @@
       <c r="X43" s="1"/>
       <c r="Y43" s="2"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" s="33" t="s">
         <v>64</v>
       </c>
@@ -3041,7 +3039,7 @@
       <c r="X44" s="1"/>
       <c r="Y44" s="2"/>
     </row>
-    <row r="45" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="33" t="s">
         <v>64</v>
       </c>
@@ -3080,7 +3078,7 @@
       <c r="X45" s="1"/>
       <c r="Y45" s="2"/>
     </row>
-    <row r="46" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A46" s="33" t="s">
         <v>64</v>
       </c>
@@ -3119,7 +3117,7 @@
       <c r="X46" s="1"/>
       <c r="Y46" s="2"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" s="33" t="s">
         <v>64</v>
       </c>
@@ -3158,7 +3156,7 @@
       <c r="X47" s="1"/>
       <c r="Y47" s="2"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48" s="33" t="s">
         <v>64</v>
       </c>
@@ -3197,7 +3195,7 @@
       <c r="X48" s="1"/>
       <c r="Y48" s="2"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A49" s="33" t="s">
         <v>64</v>
       </c>
@@ -3234,7 +3232,7 @@
       <c r="X49" s="1"/>
       <c r="Y49" s="2"/>
     </row>
-    <row r="50" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="33" t="s">
         <v>64</v>
       </c>
@@ -3273,7 +3271,7 @@
       <c r="X50" s="1"/>
       <c r="Y50" s="2"/>
     </row>
-    <row r="51" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A51" s="33" t="s">
         <v>64</v>
       </c>
@@ -3310,7 +3308,7 @@
       <c r="X51" s="1"/>
       <c r="Y51" s="2"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A52" s="39" t="s">
         <v>74</v>
       </c>
@@ -3347,7 +3345,7 @@
       <c r="X52" s="1"/>
       <c r="Y52" s="2"/>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A53" s="35" t="s">
         <v>76</v>
       </c>
@@ -3384,7 +3382,7 @@
       <c r="X53" s="1"/>
       <c r="Y53" s="2"/>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A54" s="37" t="s">
         <v>78</v>
       </c>
@@ -3394,8 +3392,12 @@
       <c r="C54" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -3417,7 +3419,7 @@
       <c r="X54" s="1"/>
       <c r="Y54" s="2"/>
     </row>
-    <row r="55" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="40" t="s">
         <v>80</v>
       </c>
@@ -3454,7 +3456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="56" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="AA3:AB3"/>
@@ -3483,12 +3485,12 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
         <v>83</v>
       </c>
@@ -3496,7 +3498,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
         <v>8</v>
       </c>
@@ -3504,7 +3506,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
@@ -3512,7 +3514,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added left and rigth, and corrected a room that you could get into but didnt exist, so you ended up in a place surrounded of nothing and couldnt go out
</commit_message>
<xml_diff>
--- a/I2_Gant_Saul_Lopez_Fernando_Mijangos.xlsx
+++ b/I2_Gant_Saul_Lopez_Fernando_Mijangos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fernandpo\cosa_uni\proyecto_program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177BF8FB-25FA-42D8-A833-F9016525845C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CC15AA-7BCD-47C6-84EF-6DFAF1E0BB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{05C49126-5558-4AD1-950B-328547F3A5DA}"/>
   </bookViews>
@@ -1289,8 +1289,8 @@
   </sheetPr>
   <dimension ref="A1:AB56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="73" workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
+      <selection activeCell="AK1" sqref="AK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2556,7 +2556,7 @@
       <c r="X31" s="1"/>
       <c r="Y31" s="2"/>
     </row>
-    <row r="32" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="23" t="s">
         <v>47</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>48</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="50" t="s">
         <v>12</v>
       </c>
       <c r="F32" s="1"/>
@@ -2577,11 +2577,11 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-      <c r="M32" s="24" t="s">
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
@@ -2593,7 +2593,7 @@
       <c r="X32" s="1"/>
       <c r="Y32" s="2"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="23" t="s">
         <v>47</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>49</v>
       </c>
       <c r="D33" s="1"/>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="50" t="s">
         <v>12</v>
       </c>
       <c r="F33" s="1"/>
@@ -2614,11 +2614,11 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-      <c r="M33" s="24" t="s">
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
@@ -2630,7 +2630,7 @@
       <c r="X33" s="1"/>
       <c r="Y33" s="2"/>
     </row>
-    <row r="34" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
bye magic numbers :(
</commit_message>
<xml_diff>
--- a/I2_Gant_Saul_Lopez_Fernando_Mijangos.xlsx
+++ b/I2_Gant_Saul_Lopez_Fernando_Mijangos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fernandpo\cosa_uni\proyecto_program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39F669D-A13D-4DD1-B714-FD0C40207C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740AF650-567F-4491-9DB6-142AF7A3DE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{05C49126-5558-4AD1-950B-328547F3A5DA}"/>
   </bookViews>
@@ -308,7 +308,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +319,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -756,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -960,6 +968,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1289,8 +1300,8 @@
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="73" workbookViewId="0">
-      <selection activeCell="W45" sqref="W45"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1299,7 +1310,8 @@
     <col min="2" max="2" width="1.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="5" style="3" customWidth="1"/>
-    <col min="6" max="25" width="2.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="14" width="2.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="25" width="3.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="26" max="27" width="10.88671875" style="3"/>
     <col min="28" max="28" width="19.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="29" max="16384" width="10.88671875" style="3"/>
@@ -1646,6 +1658,7 @@
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="2"/>
+      <c r="Z8" s="73"/>
     </row>
     <row r="9" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">

</xml_diff>

<commit_message>
and edited the excel
</commit_message>
<xml_diff>
--- a/I2_Gant_Saul_Lopez_Fernando_Mijangos.xlsx
+++ b/I2_Gant_Saul_Lopez_Fernando_Mijangos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fernandpo\cosa_uni\proyecto_program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740AF650-567F-4491-9DB6-142AF7A3DE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7825FF8-004E-47CA-8E58-EA3470928EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{05C49126-5558-4AD1-950B-328547F3A5DA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="92">
   <si>
     <t>CRONOGRAMA I2</t>
   </si>
@@ -764,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -910,6 +910,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -970,7 +973,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1300,8 +1303,8 @@
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z8" sqref="Z8"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="Q51" sqref="Q51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1318,112 +1321,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="25.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="57"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="58"/>
     </row>
     <row r="2" spans="1:28" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="64" t="s">
+      <c r="B2" s="60"/>
+      <c r="C2" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="68"/>
-      <c r="F2" s="71" t="s">
+      <c r="E2" s="69"/>
+      <c r="F2" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
-      <c r="U2" s="71"/>
-      <c r="V2" s="71"/>
-      <c r="W2" s="71"/>
-      <c r="X2" s="71"/>
-      <c r="Y2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="72"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="72"/>
+      <c r="U2" s="72"/>
+      <c r="V2" s="72"/>
+      <c r="W2" s="72"/>
+      <c r="X2" s="72"/>
+      <c r="Y2" s="73"/>
     </row>
     <row r="3" spans="1:28" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="60"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="71" t="s">
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71" t="s">
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71" t="s">
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="71"/>
-      <c r="S3" s="71"/>
-      <c r="T3" s="71"/>
-      <c r="U3" s="71" t="s">
+      <c r="Q3" s="72"/>
+      <c r="R3" s="72"/>
+      <c r="S3" s="72"/>
+      <c r="T3" s="72"/>
+      <c r="U3" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="V3" s="71"/>
-      <c r="W3" s="71"/>
-      <c r="X3" s="71"/>
-      <c r="Y3" s="72"/>
-      <c r="AA3" s="53" t="s">
+      <c r="V3" s="72"/>
+      <c r="W3" s="72"/>
+      <c r="X3" s="72"/>
+      <c r="Y3" s="73"/>
+      <c r="AA3" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="AB3" s="54"/>
+      <c r="AB3" s="55"/>
     </row>
     <row r="4" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="66"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="67"/>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1658,7 +1661,7 @@
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="2"/>
-      <c r="Z8" s="73"/>
+      <c r="Z8" s="53"/>
     </row>
     <row r="9" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
@@ -3075,7 +3078,7 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
+      <c r="O45" s="34"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
@@ -3261,7 +3264,6 @@
       <c r="N50" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="O50" s="1"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
@@ -3296,9 +3298,11 @@
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
+      <c r="O51" s="34" t="s">
+        <v>9</v>
+      </c>
       <c r="P51" s="1"/>
-      <c r="Q51" s="1"/>
+      <c r="Q51" s="74"/>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>

</xml_diff>

<commit_message>
Gant (100%) + acta dia 18 (75%)
</commit_message>
<xml_diff>
--- a/I2_Gant_Saul_Lopez_Fernando_Mijangos.xlsx
+++ b/I2_Gant_Saul_Lopez_Fernando_Mijangos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fernandpo\cosa_uni\proyecto_program\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\saul\Pprog_conversation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7825FF8-004E-47CA-8E58-EA3470928EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBA1A1B-3457-4641-B10D-F9705E85BE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{05C49126-5558-4AD1-950B-328547F3A5DA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{05C49126-5558-4AD1-950B-328547F3A5DA}"/>
   </bookViews>
   <sheets>
     <sheet name="DIAGRAMA DE GANTT" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="88">
   <si>
     <t>CRONOGRAMA I2</t>
   </si>
@@ -290,35 +290,16 @@
   </si>
   <si>
     <t>DESGLOSE</t>
-  </si>
-  <si>
-    <t>Leyenda</t>
-  </si>
-  <si>
-    <t>Objetivo a medias</t>
-  </si>
-  <si>
-    <t>Objetivo completo</t>
-  </si>
-  <si>
-    <t>Objetivo no empezado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -332,7 +313,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,12 +422,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -764,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -898,25 +873,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -971,9 +934,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1002,9 +962,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1042,7 +1002,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1148,7 +1108,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1290,7 +1250,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1303,130 +1263,128 @@
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="Q51" sqref="Q51"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="Z52" sqref="Z52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="1.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.6328125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="5" style="3" customWidth="1"/>
-    <col min="6" max="14" width="2.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="25" width="3.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="10.88671875" style="3"/>
-    <col min="28" max="28" width="19.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.88671875" style="3"/>
+    <col min="6" max="14" width="2.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="25" width="3.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="10.90625" style="3"/>
+    <col min="28" max="28" width="19.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="25.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:28" ht="26" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="58"/>
-    </row>
-    <row r="2" spans="1:28" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="59" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="54"/>
+    </row>
+    <row r="2" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="65" t="s">
+      <c r="B2" s="56"/>
+      <c r="C2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="D2" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="72" t="s">
+      <c r="E2" s="65"/>
+      <c r="F2" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="72"/>
-      <c r="R2" s="72"/>
-      <c r="S2" s="72"/>
-      <c r="T2" s="72"/>
-      <c r="U2" s="72"/>
-      <c r="V2" s="72"/>
-      <c r="W2" s="72"/>
-      <c r="X2" s="72"/>
-      <c r="Y2" s="73"/>
-    </row>
-    <row r="3" spans="1:28" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="61"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="72" t="s">
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="68"/>
+      <c r="U2" s="68"/>
+      <c r="V2" s="68"/>
+      <c r="W2" s="68"/>
+      <c r="X2" s="68"/>
+      <c r="Y2" s="69"/>
+    </row>
+    <row r="3" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="57"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72" t="s">
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72" t="s">
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="72"/>
-      <c r="S3" s="72"/>
-      <c r="T3" s="72"/>
-      <c r="U3" s="72" t="s">
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="V3" s="72"/>
-      <c r="W3" s="72"/>
-      <c r="X3" s="72"/>
-      <c r="Y3" s="73"/>
-      <c r="AA3" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB3" s="55"/>
-    </row>
-    <row r="4" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="63"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="67"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
+      <c r="X3" s="68"/>
+      <c r="Y3" s="69"/>
+      <c r="AA3"/>
+      <c r="AB3"/>
+    </row>
+    <row r="4" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="63"/>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1493,14 +1451,10 @@
       <c r="Y4" s="2">
         <v>20</v>
       </c>
-      <c r="AA4" s="49" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AA4"/>
+      <c r="AB4"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1536,14 +1490,10 @@
       <c r="W5" s="8"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="2"/>
-      <c r="AA5" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA5"/>
+      <c r="AB5"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
@@ -1554,7 +1504,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="50" t="s">
+      <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="10" t="s">
@@ -1581,14 +1531,10 @@
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="2"/>
-      <c r="AA6" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB6" s="51" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA6"/>
+      <c r="AB6"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
@@ -1598,7 +1544,7 @@
       <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="1"/>
@@ -1625,7 +1571,7 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="2"/>
     </row>
-    <row r="8" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1635,7 +1581,7 @@
       <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="1"/>
@@ -1661,9 +1607,9 @@
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="2"/>
-      <c r="Z8" s="53"/>
-    </row>
-    <row r="9" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Z8" s="50"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
@@ -1673,7 +1619,7 @@
       <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="1"/>
@@ -1700,7 +1646,7 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="2"/>
     </row>
-    <row r="10" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
@@ -1710,7 +1656,7 @@
       <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="50" t="s">
+      <c r="D10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="1"/>
@@ -1739,7 +1685,7 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>15</v>
       </c>
@@ -1749,7 +1695,7 @@
       <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="1"/>
@@ -1778,7 +1724,7 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="2"/>
     </row>
-    <row r="12" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
@@ -1788,7 +1734,7 @@
       <c r="C12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="1"/>
@@ -1819,7 +1765,7 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
@@ -1829,7 +1775,7 @@
       <c r="C13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="1"/>
@@ -1862,7 +1808,7 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="2"/>
     </row>
-    <row r="14" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>23</v>
       </c>
@@ -1873,7 +1819,7 @@
         <v>24</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="50" t="s">
+      <c r="E14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="1"/>
@@ -1901,7 +1847,7 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -1912,7 +1858,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="50" t="s">
+      <c r="E15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="1"/>
@@ -1940,7 +1886,7 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="2"/>
     </row>
-    <row r="16" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
@@ -1951,7 +1897,7 @@
         <v>26</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="50" t="s">
+      <c r="E16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="1"/>
@@ -1979,7 +1925,7 @@
       <c r="X16" s="1"/>
       <c r="Y16" s="2"/>
     </row>
-    <row r="17" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
         <v>23</v>
       </c>
@@ -1990,7 +1936,7 @@
         <v>27</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="50" t="s">
+      <c r="E17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="1"/>
@@ -2016,7 +1962,7 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>23</v>
       </c>
@@ -2027,7 +1973,7 @@
         <v>28</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="50" t="s">
+      <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="1"/>
@@ -2057,7 +2003,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
@@ -2068,7 +2014,7 @@
         <v>30</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="50" t="s">
+      <c r="E19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="1"/>
@@ -2094,7 +2040,7 @@
       <c r="X19" s="1"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>29</v>
       </c>
@@ -2105,7 +2051,7 @@
         <v>31</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="50" t="s">
+      <c r="E20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="1"/>
@@ -2155,7 +2101,7 @@
       </c>
       <c r="Y20" s="2"/>
     </row>
-    <row r="21" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>29</v>
       </c>
@@ -2166,7 +2112,7 @@
         <v>32</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="50" t="s">
+      <c r="E21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="1"/>
@@ -2192,7 +2138,7 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="2"/>
     </row>
-    <row r="22" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>29</v>
       </c>
@@ -2203,7 +2149,7 @@
         <v>33</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="50" t="s">
+      <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="1"/>
@@ -2229,7 +2175,7 @@
       <c r="X22" s="1"/>
       <c r="Y22" s="2"/>
     </row>
-    <row r="23" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>29</v>
       </c>
@@ -2240,7 +2186,7 @@
         <v>34</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="50" t="s">
+      <c r="E23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="1"/>
@@ -2266,7 +2212,7 @@
       <c r="X23" s="1"/>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>29</v>
       </c>
@@ -2277,7 +2223,7 @@
         <v>35</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="50" t="s">
+      <c r="E24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="1"/>
@@ -2303,7 +2249,7 @@
       <c r="X24" s="1"/>
       <c r="Y24" s="2"/>
     </row>
-    <row r="25" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>36</v>
       </c>
@@ -2313,7 +2259,7 @@
       <c r="C25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="50" t="s">
+      <c r="D25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="1"/>
@@ -2340,7 +2286,7 @@
       <c r="X25" s="1"/>
       <c r="Y25" s="2"/>
     </row>
-    <row r="26" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
         <v>38</v>
       </c>
@@ -2350,7 +2296,7 @@
       <c r="C26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="50" t="s">
+      <c r="D26" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="1"/>
@@ -2377,7 +2323,7 @@
       <c r="X26" s="1"/>
       <c r="Y26" s="2"/>
     </row>
-    <row r="27" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
         <v>38</v>
       </c>
@@ -2387,7 +2333,7 @@
       <c r="C27" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="50" t="s">
+      <c r="D27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E27" s="1"/>
@@ -2416,7 +2362,7 @@
       <c r="X27" s="1"/>
       <c r="Y27" s="2"/>
     </row>
-    <row r="28" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A28" s="17" t="s">
         <v>38</v>
       </c>
@@ -2426,7 +2372,7 @@
       <c r="C28" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="50" t="s">
+      <c r="D28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E28" s="1"/>
@@ -2455,20 +2401,20 @@
       <c r="X28" s="1"/>
       <c r="Y28" s="2"/>
     </row>
-    <row r="29" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
         <v>38</v>
       </c>
       <c r="B29" s="18">
         <v>4</v>
       </c>
-      <c r="C29" s="52" t="s">
+      <c r="C29" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="50" t="s">
+      <c r="D29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="1"/>
@@ -2498,7 +2444,7 @@
       <c r="X29" s="1"/>
       <c r="Y29" s="2"/>
     </row>
-    <row r="30" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A30" s="19" t="s">
         <v>43</v>
       </c>
@@ -2508,7 +2454,7 @@
       <c r="C30" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="50" t="s">
+      <c r="D30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E30" s="1"/>
@@ -2535,7 +2481,7 @@
       <c r="X30" s="1"/>
       <c r="Y30" s="2"/>
     </row>
-    <row r="31" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A31" s="21" t="s">
         <v>45</v>
       </c>
@@ -2545,7 +2491,7 @@
       <c r="C31" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="50" t="s">
+      <c r="D31" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E31" s="1"/>
@@ -2572,7 +2518,7 @@
       <c r="X31" s="1"/>
       <c r="Y31" s="2"/>
     </row>
-    <row r="32" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A32" s="23" t="s">
         <v>47</v>
       </c>
@@ -2583,7 +2529,7 @@
         <v>48</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="E32" s="50" t="s">
+      <c r="E32" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F32" s="1"/>
@@ -2609,7 +2555,7 @@
       <c r="X32" s="1"/>
       <c r="Y32" s="2"/>
     </row>
-    <row r="33" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A33" s="23" t="s">
         <v>47</v>
       </c>
@@ -2620,7 +2566,7 @@
         <v>49</v>
       </c>
       <c r="D33" s="1"/>
-      <c r="E33" s="50" t="s">
+      <c r="E33" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F33" s="1"/>
@@ -2646,7 +2592,7 @@
       <c r="X33" s="1"/>
       <c r="Y33" s="2"/>
     </row>
-    <row r="34" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
         <v>50</v>
       </c>
@@ -2656,7 +2602,7 @@
       <c r="C34" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="50" t="s">
+      <c r="D34" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E34" s="1"/>
@@ -2683,7 +2629,7 @@
       <c r="X34" s="1"/>
       <c r="Y34" s="2"/>
     </row>
-    <row r="35" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>52</v>
       </c>
@@ -2693,7 +2639,7 @@
       <c r="C35" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="50" t="s">
+      <c r="D35" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E35" s="1"/>
@@ -2720,7 +2666,7 @@
       <c r="X35" s="1"/>
       <c r="Y35" s="2"/>
     </row>
-    <row r="36" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A36" s="27" t="s">
         <v>54</v>
       </c>
@@ -2731,7 +2677,7 @@
         <v>55</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="50" t="s">
+      <c r="E36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F36" s="1"/>
@@ -2757,7 +2703,7 @@
       <c r="X36" s="1"/>
       <c r="Y36" s="2"/>
     </row>
-    <row r="37" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A37" s="29" t="s">
         <v>56</v>
       </c>
@@ -2767,7 +2713,7 @@
       <c r="C37" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="50" t="s">
+      <c r="D37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="1"/>
@@ -2794,7 +2740,7 @@
       <c r="X37" s="1"/>
       <c r="Y37" s="2"/>
     </row>
-    <row r="38" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A38" s="29" t="s">
         <v>56</v>
       </c>
@@ -2804,7 +2750,7 @@
       <c r="C38" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D38" s="50" t="s">
+      <c r="D38" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="1"/>
@@ -2831,7 +2777,7 @@
       <c r="X38" s="1"/>
       <c r="Y38" s="2"/>
     </row>
-    <row r="39" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A39" s="29" t="s">
         <v>56</v>
       </c>
@@ -2841,7 +2787,7 @@
       <c r="C39" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D39" s="50" t="s">
+      <c r="D39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E39" s="1"/>
@@ -2868,7 +2814,7 @@
       <c r="X39" s="1"/>
       <c r="Y39" s="2"/>
     </row>
-    <row r="40" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A40" s="29" t="s">
         <v>56</v>
       </c>
@@ -2878,10 +2824,10 @@
       <c r="C40" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="50" t="s">
+      <c r="D40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F40" s="1"/>
@@ -2905,7 +2851,7 @@
       <c r="X40" s="1"/>
       <c r="Y40" s="2"/>
     </row>
-    <row r="41" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A41" s="31" t="s">
         <v>61</v>
       </c>
@@ -2915,7 +2861,7 @@
       <c r="C41" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D41" s="50" t="s">
+      <c r="D41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="1"/>
@@ -2942,7 +2888,7 @@
       <c r="X41" s="1"/>
       <c r="Y41" s="2"/>
     </row>
-    <row r="42" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A42" s="31" t="s">
         <v>61</v>
       </c>
@@ -2952,7 +2898,7 @@
       <c r="C42" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="50" t="s">
+      <c r="D42" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E42" s="1"/>
@@ -2979,7 +2925,7 @@
       <c r="X42" s="1"/>
       <c r="Y42" s="2"/>
     </row>
-    <row r="43" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A43" s="33" t="s">
         <v>64</v>
       </c>
@@ -2990,7 +2936,7 @@
         <v>65</v>
       </c>
       <c r="D43" s="1"/>
-      <c r="E43" s="50" t="s">
+      <c r="E43" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F43" s="1"/>
@@ -3018,7 +2964,7 @@
       <c r="X43" s="1"/>
       <c r="Y43" s="2"/>
     </row>
-    <row r="44" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A44" s="33" t="s">
         <v>64</v>
       </c>
@@ -3029,7 +2975,7 @@
         <v>66</v>
       </c>
       <c r="D44" s="1"/>
-      <c r="E44" s="50" t="s">
+      <c r="E44" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F44" s="1"/>
@@ -3053,7 +2999,7 @@
       <c r="X44" s="1"/>
       <c r="Y44" s="2"/>
     </row>
-    <row r="45" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A45" s="33" t="s">
         <v>64</v>
       </c>
@@ -3063,7 +3009,7 @@
       <c r="C45" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="50" t="s">
+      <c r="D45" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E45" s="1" t="s">
@@ -3090,7 +3036,7 @@
       <c r="X45" s="1"/>
       <c r="Y45" s="2"/>
     </row>
-    <row r="46" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A46" s="33" t="s">
         <v>64</v>
       </c>
@@ -3101,7 +3047,7 @@
         <v>68</v>
       </c>
       <c r="D46" s="1"/>
-      <c r="E46" s="50" t="s">
+      <c r="E46" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F46" s="1"/>
@@ -3126,7 +3072,7 @@
       <c r="X46" s="1"/>
       <c r="Y46" s="2"/>
     </row>
-    <row r="47" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A47" s="33" t="s">
         <v>64</v>
       </c>
@@ -3137,7 +3083,7 @@
         <v>69</v>
       </c>
       <c r="D47" s="1"/>
-      <c r="E47" s="50" t="s">
+      <c r="E47" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F47" s="1"/>
@@ -3163,7 +3109,7 @@
       <c r="X47" s="1"/>
       <c r="Y47" s="2"/>
     </row>
-    <row r="48" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A48" s="33" t="s">
         <v>64</v>
       </c>
@@ -3174,7 +3120,7 @@
         <v>70</v>
       </c>
       <c r="D48" s="1"/>
-      <c r="E48" s="50" t="s">
+      <c r="E48" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F48" s="1"/>
@@ -3200,7 +3146,7 @@
       <c r="X48" s="1"/>
       <c r="Y48" s="2"/>
     </row>
-    <row r="49" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A49" s="33" t="s">
         <v>64</v>
       </c>
@@ -3211,7 +3157,7 @@
         <v>71</v>
       </c>
       <c r="D49" s="1"/>
-      <c r="E49" s="50" t="s">
+      <c r="E49" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F49" s="1"/>
@@ -3237,7 +3183,7 @@
       <c r="X49" s="1"/>
       <c r="Y49" s="2"/>
     </row>
-    <row r="50" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A50" s="33" t="s">
         <v>64</v>
       </c>
@@ -3247,10 +3193,10 @@
       <c r="C50" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D50" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="E50" s="50" t="s">
+      <c r="D50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F50" s="1"/>
@@ -3275,7 +3221,7 @@
       <c r="X50" s="1"/>
       <c r="Y50" s="2"/>
     </row>
-    <row r="51" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A51" s="33" t="s">
         <v>64</v>
       </c>
@@ -3286,7 +3232,7 @@
         <v>73</v>
       </c>
       <c r="D51" s="1"/>
-      <c r="E51" s="50" t="s">
+      <c r="E51" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F51" s="1"/>
@@ -3302,7 +3248,7 @@
         <v>9</v>
       </c>
       <c r="P51" s="1"/>
-      <c r="Q51" s="74"/>
+      <c r="Q51" s="51"/>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
@@ -3312,7 +3258,7 @@
       <c r="X51" s="1"/>
       <c r="Y51" s="2"/>
     </row>
-    <row r="52" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A52" s="39" t="s">
         <v>74</v>
       </c>
@@ -3349,7 +3295,7 @@
       <c r="X52" s="1"/>
       <c r="Y52" s="2"/>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A53" s="35" t="s">
         <v>76</v>
       </c>
@@ -3386,7 +3332,7 @@
       <c r="X53" s="1"/>
       <c r="Y53" s="2"/>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A54" s="37" t="s">
         <v>78</v>
       </c>
@@ -3423,7 +3369,7 @@
       <c r="X54" s="1"/>
       <c r="Y54" s="2"/>
     </row>
-    <row r="55" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="40" t="s">
         <v>80</v>
       </c>
@@ -3460,13 +3406,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="1048576" spans="16:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="1048576" spans="16:16" x14ac:dyDescent="0.35">
       <c r="P1048576" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="AA3:AB3"/>
+  <mergeCells count="9">
     <mergeCell ref="A1:Y1"/>
     <mergeCell ref="A2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -3492,12 +3437,12 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A1" s="43" t="s">
         <v>83</v>
       </c>
@@ -3505,7 +3450,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="45" t="s">
         <v>8</v>
       </c>
@@ -3513,7 +3458,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
@@ -3521,7 +3466,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>